<commit_message>
Added ability for user to set filtering on managed forms
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="83">
   <si>
     <t>name</t>
   </si>
@@ -261,6 +261,15 @@
   </si>
   <si>
     <t>and</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>Add a list box that allows the user to select a value to filter on</t>
+  </si>
+  <si>
+    <t>No filter</t>
   </si>
 </sst>
 </file>
@@ -744,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1014,11 +1023,13 @@
     <row r="29" spans="1:5">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="D29" s="2" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -1026,110 +1037,112 @@
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1"/>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1"/>
-      <c r="B35" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="D35" s="2"/>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+      <c r="D36" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1"/>
-      <c r="B37" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="D37" s="2"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38" s="2"/>
+      <c r="B38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="2" t="s">
-        <v>68</v>
-      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="2"/>
+      <c r="B40" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="5"/>
@@ -1137,44 +1150,44 @@
     <row r="42" spans="1:5">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="C42" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="D42" s="2"/>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1"/>
-      <c r="B43" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" s="6"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="2"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="6"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="2"/>
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="6"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
       <c r="E45" s="5"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1"/>
-      <c r="B46" s="6"/>
+      <c r="B46" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="C46" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="5"/>
@@ -1183,7 +1196,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="5"/>
@@ -1192,43 +1205,37 @@
       <c r="A48" s="1"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>36</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D48" s="6"/>
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D49" s="6"/>
       <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>48</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D50" s="6"/>
       <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E51" s="5"/>
     </row>
@@ -1236,10 +1243,10 @@
       <c r="A52" s="1"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E52" s="5"/>
     </row>
@@ -1247,45 +1254,78 @@
       <c r="A53" s="1"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D53" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
+      <c r="C54" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="1"/>
+      <c r="C55" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
+      <c r="C56" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="D56" s="6"/>
-      <c r="E56" s="1"/>
+      <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
       <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1299,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1310,16 +1350,16 @@
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="32.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="8" width="32.83203125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="17.6640625" style="1" customWidth="1"/>
-    <col min="11" max="13" width="10.83203125" style="1"/>
-    <col min="14" max="14" width="75.6640625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="7" width="9.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="32.83203125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="17.6640625" style="1" customWidth="1"/>
+    <col min="12" max="14" width="10.83203125" style="1"/>
+    <col min="15" max="15" width="75.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -1339,24 +1379,27 @@
         <v>63</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="K1"/>
       <c r="L1"/>
       <c r="M1"/>
       <c r="N1"/>
       <c r="O1"/>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="P1"/>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1372,13 +1415,14 @@
       <c r="M2"/>
       <c r="N2"/>
       <c r="O2"/>
-      <c r="P2" s="5"/>
+      <c r="P2"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="U2" s="5"/>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
@@ -1394,13 +1438,14 @@
       <c r="M3"/>
       <c r="N3"/>
       <c r="O3"/>
-      <c r="P3" s="5"/>
+      <c r="P3"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="U3" s="5"/>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -1416,13 +1461,14 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4"/>
-      <c r="P4" s="5"/>
+      <c r="P4"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="U4" s="5"/>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -1438,13 +1484,14 @@
       <c r="M5"/>
       <c r="N5"/>
       <c r="O5"/>
-      <c r="P5" s="5"/>
+      <c r="P5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="U5" s="5"/>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -1460,13 +1507,14 @@
       <c r="M6"/>
       <c r="N6"/>
       <c r="O6"/>
-      <c r="P6" s="5"/>
+      <c r="P6"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -1482,13 +1530,14 @@
       <c r="M7"/>
       <c r="N7"/>
       <c r="O7"/>
-      <c r="P7" s="5"/>
+      <c r="P7"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="U7" s="5"/>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -1504,13 +1553,14 @@
       <c r="M8"/>
       <c r="N8"/>
       <c r="O8"/>
-      <c r="P8" s="5"/>
+      <c r="P8"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="U8" s="5"/>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
@@ -1526,13 +1576,14 @@
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9"/>
-      <c r="P9" s="5"/>
+      <c r="P9"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="U9" s="5"/>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -1548,13 +1599,14 @@
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10"/>
-      <c r="P10" s="5"/>
+      <c r="P10"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="U10" s="5"/>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -1570,13 +1622,14 @@
       <c r="M11"/>
       <c r="N11"/>
       <c r="O11"/>
-      <c r="P11" s="5"/>
+      <c r="P11"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="U11" s="5"/>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -1592,13 +1645,14 @@
       <c r="M12"/>
       <c r="N12"/>
       <c r="O12"/>
-      <c r="P12" s="5"/>
+      <c r="P12"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="U12" s="5"/>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -1614,13 +1668,14 @@
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13"/>
-      <c r="P13" s="5"/>
+      <c r="P13"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="U13" s="5"/>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -1636,13 +1691,14 @@
       <c r="M14"/>
       <c r="N14"/>
       <c r="O14"/>
-      <c r="P14" s="5"/>
+      <c r="P14"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="U14" s="5"/>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -1658,13 +1714,14 @@
       <c r="M15"/>
       <c r="N15"/>
       <c r="O15"/>
-      <c r="P15" s="5"/>
+      <c r="P15"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="U15" s="5"/>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -1680,13 +1737,14 @@
       <c r="M16"/>
       <c r="N16"/>
       <c r="O16"/>
-      <c r="P16" s="5"/>
+      <c r="P16"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="U16" s="5"/>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -1702,399 +1760,400 @@
       <c r="M17"/>
       <c r="N17"/>
       <c r="O17"/>
-      <c r="P17" s="5"/>
+      <c r="P17"/>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="K18"/>
+      <c r="U17" s="5"/>
+    </row>
+    <row r="18" spans="1:21">
       <c r="L18"/>
       <c r="M18"/>
       <c r="N18"/>
       <c r="O18"/>
-      <c r="P18" s="5"/>
+      <c r="P18"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="K19"/>
+      <c r="U18" s="5"/>
+    </row>
+    <row r="19" spans="1:21">
       <c r="L19"/>
       <c r="M19"/>
       <c r="N19"/>
       <c r="O19"/>
-      <c r="P19" s="5"/>
+      <c r="P19"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="K20"/>
+      <c r="U19" s="5"/>
+    </row>
+    <row r="20" spans="1:21">
       <c r="L20"/>
       <c r="M20"/>
       <c r="N20"/>
       <c r="O20"/>
-      <c r="P20" s="5"/>
+      <c r="P20"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="K21"/>
+      <c r="U20" s="5"/>
+    </row>
+    <row r="21" spans="1:21">
       <c r="L21"/>
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
-      <c r="P21" s="5"/>
+      <c r="P21"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="K22"/>
+      <c r="U21" s="5"/>
+    </row>
+    <row r="22" spans="1:21">
       <c r="L22"/>
       <c r="M22"/>
       <c r="N22"/>
       <c r="O22"/>
-      <c r="P22" s="5"/>
+      <c r="P22"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="K23"/>
+      <c r="U22" s="5"/>
+    </row>
+    <row r="23" spans="1:21">
       <c r="L23"/>
       <c r="M23"/>
       <c r="N23"/>
       <c r="O23"/>
-      <c r="P23" s="5"/>
+      <c r="P23"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="K24"/>
+      <c r="U23" s="5"/>
+    </row>
+    <row r="24" spans="1:21">
       <c r="L24"/>
       <c r="M24"/>
       <c r="N24"/>
       <c r="O24"/>
-      <c r="P24" s="5"/>
+      <c r="P24"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="K25"/>
+      <c r="U24" s="5"/>
+    </row>
+    <row r="25" spans="1:21">
       <c r="L25"/>
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25"/>
-      <c r="P25" s="5"/>
+      <c r="P25"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="K26"/>
+      <c r="U25" s="5"/>
+    </row>
+    <row r="26" spans="1:21">
       <c r="L26"/>
       <c r="M26"/>
       <c r="N26"/>
       <c r="O26"/>
-      <c r="P26" s="5"/>
+      <c r="P26"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
-    </row>
-    <row r="27" spans="1:20">
-      <c r="K27"/>
+      <c r="U26" s="5"/>
+    </row>
+    <row r="27" spans="1:21">
       <c r="L27"/>
       <c r="M27"/>
       <c r="N27"/>
       <c r="O27"/>
-      <c r="P27" s="5"/>
+      <c r="P27"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
-    </row>
-    <row r="28" spans="1:20">
-      <c r="K28"/>
+      <c r="U27" s="5"/>
+    </row>
+    <row r="28" spans="1:21">
       <c r="L28"/>
       <c r="M28"/>
       <c r="N28"/>
       <c r="O28"/>
-      <c r="P28" s="5"/>
+      <c r="P28"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="K29"/>
+      <c r="U28" s="5"/>
+    </row>
+    <row r="29" spans="1:21">
       <c r="L29"/>
       <c r="M29"/>
       <c r="N29"/>
       <c r="O29"/>
-      <c r="P29" s="5"/>
+      <c r="P29"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="K30"/>
+      <c r="U29" s="5"/>
+    </row>
+    <row r="30" spans="1:21">
       <c r="L30"/>
       <c r="M30"/>
       <c r="N30"/>
       <c r="O30"/>
-      <c r="P30" s="5"/>
+      <c r="P30"/>
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="K31"/>
+      <c r="U30" s="5"/>
+    </row>
+    <row r="31" spans="1:21">
       <c r="L31"/>
       <c r="M31"/>
       <c r="N31"/>
       <c r="O31"/>
-      <c r="P31" s="5"/>
+      <c r="P31"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
-    </row>
-    <row r="32" spans="1:20">
-      <c r="K32"/>
+      <c r="U31" s="5"/>
+    </row>
+    <row r="32" spans="1:21">
       <c r="L32"/>
       <c r="M32"/>
       <c r="N32"/>
       <c r="O32"/>
-      <c r="P32" s="5"/>
+      <c r="P32"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
-    </row>
-    <row r="33" spans="11:20">
-      <c r="K33"/>
+      <c r="U32" s="5"/>
+    </row>
+    <row r="33" spans="12:21">
       <c r="L33"/>
       <c r="M33"/>
       <c r="N33"/>
       <c r="O33"/>
-      <c r="P33" s="5"/>
+      <c r="P33"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
-    </row>
-    <row r="34" spans="11:20">
-      <c r="K34"/>
+      <c r="U33" s="5"/>
+    </row>
+    <row r="34" spans="12:21">
       <c r="L34"/>
       <c r="M34"/>
       <c r="N34"/>
       <c r="O34"/>
-      <c r="P34" s="5"/>
+      <c r="P34"/>
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
-    </row>
-    <row r="35" spans="11:20">
-      <c r="K35"/>
+      <c r="U34" s="5"/>
+    </row>
+    <row r="35" spans="12:21">
       <c r="L35"/>
       <c r="M35"/>
       <c r="N35"/>
       <c r="O35"/>
-      <c r="P35" s="5"/>
+      <c r="P35"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
-    </row>
-    <row r="36" spans="11:20">
-      <c r="K36"/>
+      <c r="U35" s="5"/>
+    </row>
+    <row r="36" spans="12:21">
       <c r="L36"/>
       <c r="M36"/>
       <c r="N36"/>
       <c r="O36"/>
-      <c r="P36" s="5"/>
+      <c r="P36"/>
       <c r="Q36" s="5"/>
       <c r="R36" s="5"/>
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
-    </row>
-    <row r="37" spans="11:20">
-      <c r="K37"/>
+      <c r="U36" s="5"/>
+    </row>
+    <row r="37" spans="12:21">
       <c r="L37"/>
       <c r="M37"/>
       <c r="N37"/>
       <c r="O37"/>
-      <c r="P37" s="5"/>
+      <c r="P37"/>
       <c r="Q37" s="5"/>
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
-    </row>
-    <row r="38" spans="11:20">
-      <c r="K38"/>
+      <c r="U37" s="5"/>
+    </row>
+    <row r="38" spans="12:21">
       <c r="L38"/>
       <c r="M38"/>
       <c r="N38"/>
       <c r="O38"/>
-      <c r="P38" s="5"/>
+      <c r="P38"/>
       <c r="Q38" s="5"/>
       <c r="R38" s="5"/>
       <c r="S38" s="5"/>
       <c r="T38" s="5"/>
-    </row>
-    <row r="39" spans="11:20">
-      <c r="K39"/>
+      <c r="U38" s="5"/>
+    </row>
+    <row r="39" spans="12:21">
       <c r="L39"/>
       <c r="M39"/>
       <c r="N39"/>
       <c r="O39"/>
-      <c r="P39" s="5"/>
+      <c r="P39"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
-    </row>
-    <row r="40" spans="11:20">
-      <c r="K40"/>
+      <c r="U39" s="5"/>
+    </row>
+    <row r="40" spans="12:21">
       <c r="L40"/>
       <c r="M40"/>
       <c r="N40"/>
       <c r="O40"/>
-      <c r="P40" s="5"/>
+      <c r="P40"/>
       <c r="Q40" s="5"/>
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
-    </row>
-    <row r="41" spans="11:20">
-      <c r="K41"/>
+      <c r="U40" s="5"/>
+    </row>
+    <row r="41" spans="12:21">
       <c r="L41"/>
       <c r="M41"/>
       <c r="N41"/>
       <c r="O41"/>
-      <c r="P41" s="5"/>
+      <c r="P41"/>
       <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
       <c r="S41" s="5"/>
       <c r="T41" s="5"/>
-    </row>
-    <row r="42" spans="11:20">
-      <c r="K42"/>
+      <c r="U41" s="5"/>
+    </row>
+    <row r="42" spans="12:21">
       <c r="L42"/>
       <c r="M42"/>
       <c r="N42"/>
       <c r="O42"/>
-      <c r="P42" s="5"/>
+      <c r="P42"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
       <c r="S42" s="5"/>
       <c r="T42" s="5"/>
-    </row>
-    <row r="43" spans="11:20">
-      <c r="K43"/>
+      <c r="U42" s="5"/>
+    </row>
+    <row r="43" spans="12:21">
       <c r="L43"/>
       <c r="M43"/>
       <c r="N43"/>
       <c r="O43"/>
-      <c r="P43" s="5"/>
+      <c r="P43"/>
       <c r="Q43" s="5"/>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>
       <c r="T43" s="5"/>
-    </row>
-    <row r="44" spans="11:20">
-      <c r="K44"/>
+      <c r="U43" s="5"/>
+    </row>
+    <row r="44" spans="12:21">
       <c r="L44"/>
       <c r="M44"/>
       <c r="N44"/>
       <c r="O44"/>
-      <c r="P44" s="5"/>
+      <c r="P44"/>
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
       <c r="S44" s="5"/>
       <c r="T44" s="5"/>
-    </row>
-    <row r="45" spans="11:20">
-      <c r="K45"/>
+      <c r="U44" s="5"/>
+    </row>
+    <row r="45" spans="12:21">
       <c r="L45"/>
       <c r="M45"/>
       <c r="N45"/>
       <c r="O45"/>
-      <c r="P45" s="5"/>
+      <c r="P45"/>
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
       <c r="S45" s="5"/>
       <c r="T45" s="5"/>
-    </row>
-    <row r="46" spans="11:20">
-      <c r="K46"/>
+      <c r="U45" s="5"/>
+    </row>
+    <row r="46" spans="12:21">
       <c r="L46"/>
       <c r="M46"/>
       <c r="N46"/>
       <c r="O46"/>
-      <c r="P46" s="5"/>
+      <c r="P46"/>
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
-    </row>
-    <row r="47" spans="11:20">
-      <c r="K47"/>
+      <c r="U46" s="5"/>
+    </row>
+    <row r="47" spans="12:21">
       <c r="L47"/>
       <c r="M47"/>
       <c r="N47"/>
       <c r="O47"/>
-      <c r="P47" s="5"/>
+      <c r="P47"/>
       <c r="Q47" s="5"/>
       <c r="R47" s="5"/>
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
-    </row>
-    <row r="48" spans="11:20">
-      <c r="K48"/>
+      <c r="U47" s="5"/>
+    </row>
+    <row r="48" spans="12:21">
       <c r="L48"/>
       <c r="M48"/>
       <c r="N48"/>
       <c r="O48"/>
-    </row>
-    <row r="49" spans="11:15">
-      <c r="K49"/>
+      <c r="P48"/>
+    </row>
+    <row r="49" spans="12:16">
       <c r="L49"/>
       <c r="M49"/>
       <c r="N49"/>
       <c r="O49"/>
-    </row>
-    <row r="50" spans="11:15">
-      <c r="K50"/>
+      <c r="P49"/>
+    </row>
+    <row r="50" spans="12:16">
       <c r="L50"/>
       <c r="M50"/>
       <c r="N50"/>
       <c r="O50"/>
-    </row>
-    <row r="51" spans="11:15">
-      <c r="K51"/>
+      <c r="P50"/>
+    </row>
+    <row r="51" spans="12:16">
       <c r="L51"/>
       <c r="M51"/>
       <c r="N51"/>
       <c r="O51"/>
+      <c r="P51"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2109,10 +2168,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2120,16 +2179,16 @@
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="32.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="8" width="32.83203125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="17.6640625" style="1" customWidth="1"/>
-    <col min="11" max="13" width="10.83203125" style="1"/>
-    <col min="14" max="14" width="75.6640625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="7" width="9.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="32.83203125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="17.6640625" style="1" customWidth="1"/>
+    <col min="12" max="14" width="10.83203125" style="1"/>
+    <col min="15" max="15" width="75.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2149,24 +2208,27 @@
         <v>63</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="K1"/>
       <c r="L1"/>
       <c r="M1"/>
       <c r="N1"/>
       <c r="O1"/>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="P1"/>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2179,18 +2241,18 @@
       <c r="D2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
       <c r="N2"/>
       <c r="O2"/>
-      <c r="P2" s="5"/>
+      <c r="P2"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="U2" s="5"/>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2203,18 +2265,18 @@
       <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3"/>
       <c r="O3"/>
-      <c r="P3" s="5"/>
+      <c r="P3"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="U3" s="5"/>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2230,18 +2292,18 @@
       <c r="E4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K4"/>
       <c r="L4"/>
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4"/>
-      <c r="P4" s="5"/>
+      <c r="P4"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="U4" s="5"/>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2258,140 +2320,143 @@
         <v>61</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K5"/>
       <c r="L5"/>
       <c r="M5"/>
       <c r="N5"/>
       <c r="O5"/>
-      <c r="P5" s="5"/>
+      <c r="P5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-    </row>
-    <row r="6" spans="1:20" ht="30">
+      <c r="U5" s="5"/>
+    </row>
+    <row r="6" spans="1:21" ht="30">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
       <c r="N6"/>
       <c r="O6"/>
-      <c r="P6" s="5"/>
+      <c r="P6"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
-    </row>
-    <row r="7" spans="1:20" ht="30">
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:21" ht="30">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7"/>
       <c r="O7"/>
-      <c r="P7" s="5"/>
+      <c r="P7"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="U7" s="5"/>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
       <c r="N8"/>
       <c r="O8"/>
-      <c r="P8" s="5"/>
+      <c r="P8"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="U8" s="5"/>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K9"/>
       <c r="L9"/>
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9"/>
-      <c r="P9" s="5"/>
+      <c r="P9"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="U9" s="5"/>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K10"/>
       <c r="L10"/>
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10"/>
-      <c r="P10" s="5"/>
+      <c r="P10"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="U10" s="5"/>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -2404,18 +2469,18 @@
       <c r="D11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K11"/>
       <c r="L11"/>
       <c r="M11"/>
       <c r="N11"/>
       <c r="O11"/>
-      <c r="P11" s="5"/>
+      <c r="P11"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
-    </row>
-    <row r="12" spans="1:20" ht="45">
+      <c r="U11" s="5"/>
+    </row>
+    <row r="12" spans="1:21" ht="45">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -2428,54 +2493,54 @@
       <c r="D12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K12"/>
       <c r="L12"/>
       <c r="M12"/>
       <c r="N12"/>
       <c r="O12"/>
-      <c r="P12" s="5"/>
+      <c r="P12"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="U12" s="5"/>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="K13"/>
       <c r="L13"/>
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13"/>
-      <c r="P13" s="5"/>
+      <c r="P13"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
-    </row>
-    <row r="14" spans="1:20" ht="30">
+      <c r="U13" s="5"/>
+    </row>
+    <row r="14" spans="1:21" ht="30">
       <c r="A14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K14"/>
       <c r="L14"/>
       <c r="M14"/>
       <c r="N14"/>
       <c r="O14"/>
-      <c r="P14" s="5"/>
+      <c r="P14"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="U14" s="5"/>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -2488,428 +2553,428 @@
       <c r="D15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K15"/>
       <c r="L15"/>
       <c r="M15"/>
       <c r="N15"/>
       <c r="O15"/>
-      <c r="P15" s="5"/>
+      <c r="P15"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="K16"/>
+      <c r="U15" s="5"/>
+    </row>
+    <row r="16" spans="1:21">
       <c r="L16"/>
       <c r="M16"/>
       <c r="N16"/>
       <c r="O16"/>
-      <c r="P16" s="5"/>
+      <c r="P16"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
-    </row>
-    <row r="17" spans="11:20">
-      <c r="K17"/>
+      <c r="U16" s="5"/>
+    </row>
+    <row r="17" spans="12:21">
       <c r="L17"/>
       <c r="M17"/>
       <c r="N17"/>
       <c r="O17"/>
-      <c r="P17" s="5"/>
+      <c r="P17"/>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
-    </row>
-    <row r="18" spans="11:20">
-      <c r="K18"/>
+      <c r="U17" s="5"/>
+    </row>
+    <row r="18" spans="12:21">
       <c r="L18"/>
       <c r="M18"/>
       <c r="N18"/>
       <c r="O18"/>
-      <c r="P18" s="5"/>
+      <c r="P18"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
-    </row>
-    <row r="19" spans="11:20">
-      <c r="K19"/>
+      <c r="U18" s="5"/>
+    </row>
+    <row r="19" spans="12:21">
       <c r="L19"/>
       <c r="M19"/>
       <c r="N19"/>
       <c r="O19"/>
-      <c r="P19" s="5"/>
+      <c r="P19"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
-    </row>
-    <row r="20" spans="11:20">
-      <c r="K20"/>
+      <c r="U19" s="5"/>
+    </row>
+    <row r="20" spans="12:21">
       <c r="L20"/>
       <c r="M20"/>
       <c r="N20"/>
       <c r="O20"/>
-      <c r="P20" s="5"/>
+      <c r="P20"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
-    </row>
-    <row r="21" spans="11:20">
-      <c r="K21"/>
+      <c r="U20" s="5"/>
+    </row>
+    <row r="21" spans="12:21">
       <c r="L21"/>
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
-      <c r="P21" s="5"/>
+      <c r="P21"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
-    </row>
-    <row r="22" spans="11:20">
-      <c r="K22"/>
+      <c r="U21" s="5"/>
+    </row>
+    <row r="22" spans="12:21">
       <c r="L22"/>
       <c r="M22"/>
       <c r="N22"/>
       <c r="O22"/>
-      <c r="P22" s="5"/>
+      <c r="P22"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
-    </row>
-    <row r="23" spans="11:20">
-      <c r="K23"/>
+      <c r="U22" s="5"/>
+    </row>
+    <row r="23" spans="12:21">
       <c r="L23"/>
       <c r="M23"/>
       <c r="N23"/>
       <c r="O23"/>
-      <c r="P23" s="5"/>
+      <c r="P23"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
-    </row>
-    <row r="24" spans="11:20">
-      <c r="K24"/>
+      <c r="U23" s="5"/>
+    </row>
+    <row r="24" spans="12:21">
       <c r="L24"/>
       <c r="M24"/>
       <c r="N24"/>
       <c r="O24"/>
-      <c r="P24" s="5"/>
+      <c r="P24"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
-    </row>
-    <row r="25" spans="11:20">
-      <c r="K25"/>
+      <c r="U24" s="5"/>
+    </row>
+    <row r="25" spans="12:21">
       <c r="L25"/>
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25"/>
-      <c r="P25" s="5"/>
+      <c r="P25"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
-    </row>
-    <row r="26" spans="11:20">
-      <c r="K26"/>
+      <c r="U25" s="5"/>
+    </row>
+    <row r="26" spans="12:21">
       <c r="L26"/>
       <c r="M26"/>
       <c r="N26"/>
       <c r="O26"/>
-      <c r="P26" s="5"/>
+      <c r="P26"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
-    </row>
-    <row r="27" spans="11:20">
-      <c r="K27"/>
+      <c r="U26" s="5"/>
+    </row>
+    <row r="27" spans="12:21">
       <c r="L27"/>
       <c r="M27"/>
       <c r="N27"/>
       <c r="O27"/>
-      <c r="P27" s="5"/>
+      <c r="P27"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
-    </row>
-    <row r="28" spans="11:20">
-      <c r="K28"/>
+      <c r="U27" s="5"/>
+    </row>
+    <row r="28" spans="12:21">
       <c r="L28"/>
       <c r="M28"/>
       <c r="N28"/>
       <c r="O28"/>
-      <c r="P28" s="5"/>
+      <c r="P28"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
-    </row>
-    <row r="29" spans="11:20">
-      <c r="K29"/>
+      <c r="U28" s="5"/>
+    </row>
+    <row r="29" spans="12:21">
       <c r="L29"/>
       <c r="M29"/>
       <c r="N29"/>
       <c r="O29"/>
-      <c r="P29" s="5"/>
+      <c r="P29"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
-    </row>
-    <row r="30" spans="11:20">
-      <c r="K30"/>
+      <c r="U29" s="5"/>
+    </row>
+    <row r="30" spans="12:21">
       <c r="L30"/>
       <c r="M30"/>
       <c r="N30"/>
       <c r="O30"/>
-      <c r="P30" s="5"/>
+      <c r="P30"/>
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
-    </row>
-    <row r="31" spans="11:20">
-      <c r="K31"/>
+      <c r="U30" s="5"/>
+    </row>
+    <row r="31" spans="12:21">
       <c r="L31"/>
       <c r="M31"/>
       <c r="N31"/>
       <c r="O31"/>
-      <c r="P31" s="5"/>
+      <c r="P31"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
-    </row>
-    <row r="32" spans="11:20">
-      <c r="K32"/>
+      <c r="U31" s="5"/>
+    </row>
+    <row r="32" spans="12:21">
       <c r="L32"/>
       <c r="M32"/>
       <c r="N32"/>
       <c r="O32"/>
-      <c r="P32" s="5"/>
+      <c r="P32"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
-    </row>
-    <row r="33" spans="11:20">
-      <c r="K33"/>
+      <c r="U32" s="5"/>
+    </row>
+    <row r="33" spans="12:21">
       <c r="L33"/>
       <c r="M33"/>
       <c r="N33"/>
       <c r="O33"/>
-      <c r="P33" s="5"/>
+      <c r="P33"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
-    </row>
-    <row r="34" spans="11:20">
-      <c r="K34"/>
+      <c r="U33" s="5"/>
+    </row>
+    <row r="34" spans="12:21">
       <c r="L34"/>
       <c r="M34"/>
       <c r="N34"/>
       <c r="O34"/>
-      <c r="P34" s="5"/>
+      <c r="P34"/>
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
-    </row>
-    <row r="35" spans="11:20">
-      <c r="K35"/>
+      <c r="U34" s="5"/>
+    </row>
+    <row r="35" spans="12:21">
       <c r="L35"/>
       <c r="M35"/>
       <c r="N35"/>
       <c r="O35"/>
-      <c r="P35" s="5"/>
+      <c r="P35"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
-    </row>
-    <row r="36" spans="11:20">
-      <c r="K36"/>
+      <c r="U35" s="5"/>
+    </row>
+    <row r="36" spans="12:21">
       <c r="L36"/>
       <c r="M36"/>
       <c r="N36"/>
       <c r="O36"/>
-      <c r="P36" s="5"/>
+      <c r="P36"/>
       <c r="Q36" s="5"/>
       <c r="R36" s="5"/>
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
-    </row>
-    <row r="37" spans="11:20">
-      <c r="K37"/>
+      <c r="U36" s="5"/>
+    </row>
+    <row r="37" spans="12:21">
       <c r="L37"/>
       <c r="M37"/>
       <c r="N37"/>
       <c r="O37"/>
-      <c r="P37" s="5"/>
+      <c r="P37"/>
       <c r="Q37" s="5"/>
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
-    </row>
-    <row r="38" spans="11:20">
-      <c r="K38"/>
+      <c r="U37" s="5"/>
+    </row>
+    <row r="38" spans="12:21">
       <c r="L38"/>
       <c r="M38"/>
       <c r="N38"/>
       <c r="O38"/>
-      <c r="P38" s="5"/>
+      <c r="P38"/>
       <c r="Q38" s="5"/>
       <c r="R38" s="5"/>
       <c r="S38" s="5"/>
       <c r="T38" s="5"/>
-    </row>
-    <row r="39" spans="11:20">
-      <c r="K39"/>
+      <c r="U38" s="5"/>
+    </row>
+    <row r="39" spans="12:21">
       <c r="L39"/>
       <c r="M39"/>
       <c r="N39"/>
       <c r="O39"/>
-      <c r="P39" s="5"/>
+      <c r="P39"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
-    </row>
-    <row r="40" spans="11:20">
-      <c r="K40"/>
+      <c r="U39" s="5"/>
+    </row>
+    <row r="40" spans="12:21">
       <c r="L40"/>
       <c r="M40"/>
       <c r="N40"/>
       <c r="O40"/>
-      <c r="P40" s="5"/>
+      <c r="P40"/>
       <c r="Q40" s="5"/>
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
-    </row>
-    <row r="41" spans="11:20">
-      <c r="K41"/>
+      <c r="U40" s="5"/>
+    </row>
+    <row r="41" spans="12:21">
       <c r="L41"/>
       <c r="M41"/>
       <c r="N41"/>
       <c r="O41"/>
-      <c r="P41" s="5"/>
+      <c r="P41"/>
       <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
       <c r="S41" s="5"/>
       <c r="T41" s="5"/>
-    </row>
-    <row r="42" spans="11:20">
-      <c r="K42"/>
+      <c r="U41" s="5"/>
+    </row>
+    <row r="42" spans="12:21">
       <c r="L42"/>
       <c r="M42"/>
       <c r="N42"/>
       <c r="O42"/>
-      <c r="P42" s="5"/>
+      <c r="P42"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
       <c r="S42" s="5"/>
       <c r="T42" s="5"/>
-    </row>
-    <row r="43" spans="11:20">
-      <c r="K43"/>
+      <c r="U42" s="5"/>
+    </row>
+    <row r="43" spans="12:21">
       <c r="L43"/>
       <c r="M43"/>
       <c r="N43"/>
       <c r="O43"/>
-      <c r="P43" s="5"/>
+      <c r="P43"/>
       <c r="Q43" s="5"/>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>
       <c r="T43" s="5"/>
-    </row>
-    <row r="44" spans="11:20">
-      <c r="K44"/>
+      <c r="U43" s="5"/>
+    </row>
+    <row r="44" spans="12:21">
       <c r="L44"/>
       <c r="M44"/>
       <c r="N44"/>
       <c r="O44"/>
-      <c r="P44" s="5"/>
+      <c r="P44"/>
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
       <c r="S44" s="5"/>
       <c r="T44" s="5"/>
-    </row>
-    <row r="45" spans="11:20">
-      <c r="K45"/>
+      <c r="U44" s="5"/>
+    </row>
+    <row r="45" spans="12:21">
       <c r="L45"/>
       <c r="M45"/>
       <c r="N45"/>
       <c r="O45"/>
-      <c r="P45" s="5"/>
+      <c r="P45"/>
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
       <c r="S45" s="5"/>
       <c r="T45" s="5"/>
-    </row>
-    <row r="46" spans="11:20">
-      <c r="K46"/>
+      <c r="U45" s="5"/>
+    </row>
+    <row r="46" spans="12:21">
       <c r="L46"/>
       <c r="M46"/>
       <c r="N46"/>
       <c r="O46"/>
-      <c r="P46" s="5"/>
+      <c r="P46"/>
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
-    </row>
-    <row r="47" spans="11:20">
-      <c r="K47"/>
+      <c r="U46" s="5"/>
+    </row>
+    <row r="47" spans="12:21">
       <c r="L47"/>
       <c r="M47"/>
       <c r="N47"/>
       <c r="O47"/>
-      <c r="P47" s="5"/>
+      <c r="P47"/>
       <c r="Q47" s="5"/>
       <c r="R47" s="5"/>
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
-    </row>
-    <row r="48" spans="11:20">
-      <c r="K48"/>
+      <c r="U47" s="5"/>
+    </row>
+    <row r="48" spans="12:21">
       <c r="L48"/>
       <c r="M48"/>
       <c r="N48"/>
       <c r="O48"/>
-    </row>
-    <row r="49" spans="11:15">
-      <c r="K49"/>
+      <c r="P48"/>
+    </row>
+    <row r="49" spans="12:16">
       <c r="L49"/>
       <c r="M49"/>
       <c r="N49"/>
       <c r="O49"/>
-    </row>
-    <row r="50" spans="11:15">
-      <c r="K50"/>
+      <c r="P49"/>
+    </row>
+    <row r="50" spans="12:16">
       <c r="L50"/>
       <c r="M50"/>
       <c r="N50"/>
       <c r="O50"/>
-    </row>
-    <row r="51" spans="11:15">
-      <c r="K51"/>
+      <c r="P50"/>
+    </row>
+    <row r="51" spans="12:16">
       <c r="L51"/>
       <c r="M51"/>
       <c r="N51"/>
       <c r="O51"/>
+      <c r="P51"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Starting to add expressions to manage forms
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="13660" tabRatio="500"/>
+    <workbookView xWindow="7560" yWindow="440" windowWidth="25120" windowHeight="13660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="89">
   <si>
     <t>name</t>
   </si>
@@ -158,9 +158,6 @@
     <t>expression</t>
   </si>
   <si>
-    <t>An expression, see below for what can be included in an expresion</t>
-  </si>
-  <si>
     <t xml:space="preserve">text  </t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>Action Taken</t>
   </si>
   <si>
-    <t>The name of the column, starts with an underscore, has no spaces and only contains latin alphabet characters and numerals. Must be less than 60 characters long.</t>
-  </si>
-  <si>
     <t>_mgmt_address_recommendation</t>
   </si>
   <si>
@@ -270,6 +264,30 @@
   </si>
   <si>
     <t>No filter</t>
+  </si>
+  <si>
+    <t>The name of the column, has no spaces and only contains english alphabet characters and numerals. Must be less than 60 characters long.</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Subtracts</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Adds</t>
+  </si>
+  <si>
+    <t>An expression, see below for what can be included in an expresion. Write the expression in the condition column.</t>
   </si>
 </sst>
 </file>
@@ -753,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -853,10 +871,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E10" s="5"/>
     </row>
@@ -900,26 +918,26 @@
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5">
       <c r="A16" s="1"/>
-      <c r="B16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5"/>
     </row>
@@ -930,11 +948,15 @@
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="30">
       <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5">
@@ -944,15 +966,11 @@
       <c r="D20" s="2"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="30">
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
-      <c r="B21" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5">
@@ -962,26 +980,22 @@
       <c r="D22" s="2"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:5">
       <c r="A23" s="1"/>
-      <c r="B23" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5">
@@ -991,16 +1005,16 @@
       <c r="D25" s="2"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="30">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E26" s="5"/>
     </row>
@@ -1008,7 +1022,7 @@
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="5"/>
@@ -1023,13 +1037,13 @@
     <row r="29" spans="1:5">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -1037,11 +1051,9 @@
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5">
@@ -1054,11 +1066,13 @@
     <row r="32" spans="1:5">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D32" s="2" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -1066,110 +1080,112 @@
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1"/>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" ht="30">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1"/>
-      <c r="B38" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="D38" s="2"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
+      <c r="B39" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1"/>
-      <c r="B40" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="D40" s="2"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D41" s="2"/>
+      <c r="B41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
-      <c r="C42" s="2" t="s">
-        <v>68</v>
-      </c>
+      <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="2"/>
+      <c r="B43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="5"/>
@@ -1177,44 +1193,44 @@
     <row r="45" spans="1:5">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="C45" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="D45" s="2"/>
       <c r="E45" s="5"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1"/>
-      <c r="B46" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D46" s="6"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" s="2"/>
       <c r="E46" s="5"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D47" s="6"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="2"/>
       <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D48" s="6"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1"/>
-      <c r="B49" s="6"/>
+      <c r="B49" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="C49" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="5"/>
@@ -1223,7 +1239,7 @@
       <c r="A50" s="1"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="5"/>
@@ -1232,43 +1248,37 @@
       <c r="A51" s="1"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>36</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D51" s="6"/>
       <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D52" s="6"/>
       <c r="E52" s="5"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>48</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D53" s="6"/>
       <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E54" s="5"/>
     </row>
@@ -1276,10 +1286,10 @@
       <c r="A55" s="1"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E55" s="5"/>
     </row>
@@ -1287,45 +1297,86 @@
       <c r="A56" s="1"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D56" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
+      <c r="C57" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="1"/>
+      <c r="C58" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E58" s="5"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
+      <c r="C59" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="D59" s="6"/>
-      <c r="E59" s="1"/>
+      <c r="E59" s="5"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E60" s="5"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>87</v>
+      </c>
       <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="1"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1373,13 +1424,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -1391,7 +1442,7 @@
         <v>29</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
@@ -2202,13 +2253,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -2220,7 +2271,7 @@
         <v>29</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
@@ -2290,7 +2341,7 @@
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L4"/>
       <c r="M4"/>
@@ -2317,10 +2368,10 @@
         <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
@@ -2347,7 +2398,7 @@
         <v>40</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L6"/>
       <c r="M6"/>
@@ -2371,7 +2422,7 @@
         <v>39</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L7"/>
       <c r="M7"/>
@@ -2395,7 +2446,7 @@
         <v>42</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L8"/>
       <c r="M8"/>
@@ -2413,13 +2464,13 @@
         <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -2437,13 +2488,13 @@
         <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L10"/>
       <c r="M10"/>
@@ -2464,10 +2515,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="L11"/>
       <c r="M11"/>
@@ -2485,13 +2536,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L12"/>
       <c r="M12"/>
@@ -2506,10 +2557,10 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>73</v>
       </c>
       <c r="L13"/>
       <c r="M13"/>
@@ -2524,10 +2575,10 @@
     </row>
     <row r="14" spans="1:21" ht="30">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L14"/>
       <c r="M14"/>
@@ -2548,7 +2599,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
add support for brackets in calculations
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="440" windowWidth="25120" windowHeight="13660" tabRatio="500"/>
+    <workbookView xWindow="2900" yWindow="920" windowWidth="25120" windowHeight="13660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="93">
   <si>
     <t>name</t>
   </si>
@@ -278,16 +278,28 @@
     <t>-</t>
   </si>
   <si>
-    <t>Subtracts</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
-    <t>Adds</t>
-  </si>
-  <si>
     <t>An expression, see below for what can be included in an expresion. Write the expression in the condition column.</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Subtract</t>
+  </si>
+  <si>
+    <t>Multiply</t>
+  </si>
+  <si>
+    <t>Divide</t>
   </si>
 </sst>
 </file>
@@ -356,8 +368,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -415,7 +431,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -429,6 +445,8 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -442,6 +460,8 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -771,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1123,7 +1143,7 @@
         <v>44</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -1339,47 +1359,49 @@
       <c r="A60" s="1"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E60" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E61" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="1"/>
+      <c r="C62" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E62" s="5"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E63" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Add checking for smap meta reserved words when creating a new column.
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="920" windowWidth="25120" windowHeight="13660" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="2540" windowWidth="25120" windowHeight="13780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -266,9 +266,6 @@
     <t>No filter</t>
   </si>
   <si>
-    <t>The name of the column, has no spaces and only contains english alphabet characters and numerals. Must be less than 60 characters long.</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -300,6 +297,10 @@
   </si>
   <si>
     <t>Divide</t>
+  </si>
+  <si>
+    <t>The name of the column, has no spaces and only contains english alphabet characters and numerals. Must be less than 60 characters long.
+The following names cannot be used: _hrk, instanceid, _instanceid, _start, _end,_device, prikey, parkey, _bad, _bad_reason, _user, _survey_notes, _upload_time, _s_id, _version, _complete, _location_trigger, _modified, _task_key, _task_replace</t>
   </si>
 </sst>
 </file>
@@ -793,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -947,7 +948,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="5"/>
@@ -956,7 +957,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5"/>
@@ -968,14 +969,14 @@
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="30">
+    <row r="19" spans="1:5" ht="75">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="E19" s="5"/>
     </row>
@@ -1143,7 +1144,7 @@
         <v>44</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -1359,10 +1360,10 @@
       <c r="A60" s="1"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E60" s="1"/>
     </row>
@@ -1370,10 +1371,10 @@
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E61" s="5"/>
     </row>
@@ -1381,10 +1382,10 @@
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E62" s="5"/>
     </row>
@@ -1392,10 +1393,10 @@
       <c r="A63" s="1"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E63" s="5"/>
     </row>

</xml_diff>

<commit_message>
add translations.  Refresh survey list in managed forms when project changes
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="2540" windowWidth="25120" windowHeight="13780" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="13380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="94">
   <si>
     <t>name</t>
   </si>
@@ -278,9 +278,6 @@
     <t>+</t>
   </si>
   <si>
-    <t>An expression, see below for what can be included in an expresion. Write the expression in the condition column.</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -300,7 +297,14 @@
   </si>
   <si>
     <t>The name of the column, has no spaces and only contains english alphabet characters and numerals. Must be less than 60 characters long.
-The following names cannot be used: _hrk, instanceid, _instanceid, _start, _end,_device, prikey, parkey, _bad, _bad_reason, _user, _survey_notes, _upload_time, _s_id, _version, _complete, _location_trigger, _modified, _task_key, _task_replace</t>
+The following names cannot be used: _hrk, instanceid, _instanceid, _start, _end,_device, prikey, parkey, _bad, _bad_reason, _user, _survey_notes, _upload_time, _s_id, _version, _complete, _location_trigger, _modified, _task_key, _task_replace
+In addition you can't use sql reserved words such as "select".  However don't worry about these restricted names, you will get an error message if you upload a file that contains a name that is not accepted.</t>
+  </si>
+  <si>
+    <t>an expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An expression, see below for what can be included in an expresion. </t>
   </si>
 </sst>
 </file>
@@ -794,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -969,14 +973,14 @@
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="75">
+    <row r="19" spans="1:5" ht="150">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E19" s="5"/>
     </row>
@@ -1141,10 +1145,10 @@
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -1363,7 +1367,7 @@
         <v>84</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E60" s="1"/>
     </row>
@@ -1374,7 +1378,7 @@
         <v>83</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E61" s="5"/>
     </row>
@@ -1382,10 +1386,10 @@
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E62" s="5"/>
     </row>
@@ -1393,10 +1397,10 @@
       <c r="A63" s="1"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E63" s="5"/>
     </row>

</xml_diff>

<commit_message>
Fix issue with updating select_one managed forms types
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="95">
   <si>
     <t>name</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t xml:space="preserve">An expression, see below for what can be included in an expresion. </t>
+  </si>
+  <si>
+    <t>All of the following tokens should be separated by spaces. For exampe ( 100 + 5 ) / 10</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -434,6 +437,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="31">
@@ -796,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1251,20 +1257,20 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1"/>
-      <c r="B49" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="10"/>
       <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1"/>
-      <c r="B50" s="6"/>
+      <c r="B50" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="C50" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="5"/>
@@ -1273,7 +1279,7 @@
       <c r="A51" s="1"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="5"/>
@@ -1291,7 +1297,7 @@
       <c r="A53" s="1"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="5"/>
@@ -1300,21 +1306,19 @@
       <c r="A54" s="1"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D54" s="6"/>
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E55" s="5"/>
     </row>
@@ -1322,10 +1326,10 @@
       <c r="A56" s="1"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E56" s="5"/>
     </row>
@@ -1333,10 +1337,10 @@
       <c r="A57" s="1"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E57" s="5"/>
     </row>
@@ -1344,10 +1348,10 @@
       <c r="A58" s="1"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E58" s="5"/>
     </row>
@@ -1355,41 +1359,41 @@
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D59" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="E59" s="5"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E60" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="D60" s="6"/>
+      <c r="E60" s="5"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E61" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E62" s="5"/>
     </row>
@@ -1397,14 +1401,28 @@
       <c r="A63" s="1"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E63" s="5"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D64" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E63" s="5"/>
+      <c r="E64" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C49:D49"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Fix issue with condition failing if it its the last option in a managed form
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="13380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -140,18 +140,9 @@
     <t>${_mgmt_action_deadline} &lt; ${_mgmt_action_date}</t>
   </si>
   <si>
-    <t>'Done with delay'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Deadline Met'</t>
-  </si>
-  <si>
     <t>${_mgmt_action_deadline} &gt; now()</t>
   </si>
   <si>
-    <t xml:space="preserve"> 'In the pipeline'</t>
-  </si>
-  <si>
     <t>now()</t>
   </si>
   <si>
@@ -171,9 +162,6 @@
   </si>
   <si>
     <t>${_mgmt_action_deadline} is empty</t>
-  </si>
-  <si>
-    <t>'Deadline crossed'</t>
   </si>
   <si>
     <t>all</t>
@@ -308,6 +296,18 @@
   </si>
   <si>
     <t>All of the following tokens should be separated by spaces. For exampe ( 100 + 5 ) / 10</t>
+  </si>
+  <si>
+    <t>Deadline Met</t>
+  </si>
+  <si>
+    <t>Done with delay</t>
+  </si>
+  <si>
+    <t>In the pipeline</t>
+  </si>
+  <si>
+    <t>Deadline crossed</t>
   </si>
 </sst>
 </file>
@@ -804,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
@@ -902,10 +902,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E10" s="5"/>
     </row>
@@ -949,7 +949,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="5"/>
@@ -958,7 +958,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="5"/>
@@ -967,7 +967,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5"/>
@@ -986,7 +986,7 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E19" s="5"/>
     </row>
@@ -1039,13 +1039,13 @@
     <row r="26" spans="1:5" ht="30">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="E26" s="5"/>
     </row>
@@ -1053,7 +1053,7 @@
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="5"/>
@@ -1068,13 +1068,13 @@
     <row r="29" spans="1:5">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -1082,7 +1082,7 @@
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="5"/>
@@ -1097,13 +1097,13 @@
     <row r="32" spans="1:5">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -1111,10 +1111,10 @@
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -1151,10 +1151,10 @@
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E41" s="5"/>
     </row>
@@ -1204,11 +1204,11 @@
     <row r="43" spans="1:5">
       <c r="A43" s="1"/>
       <c r="B43" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -1216,7 +1216,7 @@
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="5"/>
@@ -1225,7 +1225,7 @@
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="5"/>
@@ -1234,7 +1234,7 @@
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="5"/>
@@ -1243,7 +1243,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="5"/>
@@ -1259,7 +1259,7 @@
       <c r="A49" s="1"/>
       <c r="B49" s="6"/>
       <c r="C49" s="10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="5"/>
@@ -1267,7 +1267,7 @@
     <row r="50" spans="1:5">
       <c r="A50" s="1"/>
       <c r="B50" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>32</v>
@@ -1315,7 +1315,7 @@
       <c r="A55" s="1"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>36</v>
@@ -1326,7 +1326,7 @@
       <c r="A56" s="1"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>37</v>
@@ -1337,10 +1337,10 @@
       <c r="A57" s="1"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E57" s="5"/>
     </row>
@@ -1348,10 +1348,10 @@
       <c r="A58" s="1"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E58" s="5"/>
     </row>
@@ -1359,10 +1359,10 @@
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E59" s="5"/>
     </row>
@@ -1370,7 +1370,7 @@
       <c r="A60" s="1"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="5"/>
@@ -1379,10 +1379,10 @@
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E61" s="1"/>
     </row>
@@ -1390,10 +1390,10 @@
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E62" s="5"/>
     </row>
@@ -1401,10 +1401,10 @@
       <c r="A63" s="1"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="E63" s="5"/>
     </row>
@@ -1412,10 +1412,10 @@
       <c r="A64" s="1"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="E64" s="5"/>
     </row>
@@ -1469,13 +1469,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -1487,7 +1487,7 @@
         <v>29</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
@@ -2266,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2298,13 +2298,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -2316,7 +2316,7 @@
         <v>29</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
@@ -2386,7 +2386,7 @@
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L4"/>
       <c r="M4"/>
@@ -2413,10 +2413,10 @@
         <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
@@ -2440,10 +2440,10 @@
         <v>31</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L6"/>
       <c r="M6"/>
@@ -2464,10 +2464,10 @@
         <v>38</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L7"/>
       <c r="M7"/>
@@ -2485,13 +2485,13 @@
         <v>10</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L8"/>
       <c r="M8"/>
@@ -2509,13 +2509,13 @@
         <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -2533,13 +2533,13 @@
         <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L10"/>
       <c r="M10"/>
@@ -2560,10 +2560,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="L11"/>
       <c r="M11"/>
@@ -2581,13 +2581,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L12"/>
       <c r="M12"/>
@@ -2602,10 +2602,10 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="L13"/>
       <c r="M13"/>
@@ -2620,10 +2620,10 @@
     </row>
     <row r="14" spans="1:21" ht="30">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L14"/>
       <c r="M14"/>
@@ -2644,7 +2644,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Addition of user role to smap server.  Started adding processing of user_role setting in oversight template
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="97">
   <si>
     <t>name</t>
   </si>
@@ -308,6 +308,12 @@
   </si>
   <si>
     <t>Deadline crossed</t>
+  </si>
+  <si>
+    <t>user_role</t>
+  </si>
+  <si>
+    <t>If used after a select_one then the list of choices will be the users on the system that have the specified role.  Multiple rows with different roles can be added.</t>
   </si>
 </sst>
 </file>
@@ -802,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -909,29 +915,31 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="30">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="5"/>
@@ -940,7 +948,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="5"/>
@@ -949,7 +957,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="5"/>
@@ -958,7 +966,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="5"/>
@@ -967,7 +975,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5"/>
@@ -975,26 +983,28 @@
     <row r="18" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="150">
+    <row r="19" spans="1:5">
       <c r="A19" s="1"/>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" ht="150">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5">
@@ -1018,214 +1028,212 @@
       <c r="D23" s="2"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5">
       <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="30">
+    <row r="26" spans="1:5">
       <c r="A26" s="1"/>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" ht="30">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="2"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1"/>
-      <c r="B29" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="C30" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1"/>
-      <c r="B32" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="C33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1"/>
-      <c r="B35" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="D35" s="2"/>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" ht="30">
+    <row r="37" spans="1:5">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" ht="30">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="C38" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1"/>
-      <c r="B39" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="D39" s="2"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
+      <c r="B40" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="D40" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1"/>
-      <c r="B41" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="D41" s="2"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1"/>
-      <c r="B42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1"/>
-      <c r="B43" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="D43" s="2"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" s="2"/>
+      <c r="B44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="5"/>
@@ -1234,7 +1242,7 @@
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="5"/>
@@ -1243,7 +1251,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="5"/>
@@ -1251,35 +1259,35 @@
     <row r="48" spans="1:5">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="D48" s="2"/>
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D49" s="10"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
       <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1"/>
-      <c r="B50" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" s="10"/>
       <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1"/>
-      <c r="B51" s="6"/>
+      <c r="B51" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="C51" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="5"/>
@@ -1288,7 +1296,7 @@
       <c r="A52" s="1"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="5"/>
@@ -1306,7 +1314,7 @@
       <c r="A54" s="1"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
@@ -1315,21 +1323,19 @@
       <c r="A55" s="1"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D55" s="6"/>
       <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E56" s="5"/>
     </row>
@@ -1337,10 +1343,10 @@
       <c r="A57" s="1"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E57" s="5"/>
     </row>
@@ -1348,10 +1354,10 @@
       <c r="A58" s="1"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E58" s="5"/>
     </row>
@@ -1359,10 +1365,10 @@
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E59" s="5"/>
     </row>
@@ -1370,41 +1376,41 @@
       <c r="A60" s="1"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D60" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="E60" s="5"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E61" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="D61" s="6"/>
+      <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E62" s="5"/>
+        <v>83</v>
+      </c>
+      <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E63" s="5"/>
     </row>
@@ -1412,16 +1418,27 @@
       <c r="A64" s="1"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E64" s="5"/>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="1"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D65" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E64" s="5"/>
+      <c r="E65" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2266,7 +2283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add ability to select from a list of users in managed forms
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="97">
   <si>
     <t>name</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Comment</t>
-  </si>
-  <si>
-    <t>The name to be shown at the top of the colum in the report.  Can be any value.</t>
   </si>
   <si>
     <t>Contains the calculation if the data type is "calculate"</t>
@@ -314,6 +311,9 @@
   </si>
   <si>
     <t>If used after a select_one then the list of choices will be the users on the system that have the specified role.  Multiple rows with different roles can be added.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name to be shown at the top of the colum in the report.  Can be any value. </t>
   </si>
 </sst>
 </file>
@@ -382,8 +382,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -448,7 +450,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -464,6 +466,7 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -479,6 +482,7 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -810,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -908,10 +912,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="E10" s="5"/>
     </row>
@@ -919,10 +923,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="E11" s="5"/>
     </row>
@@ -948,7 +952,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="5"/>
@@ -957,7 +961,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="5"/>
@@ -966,7 +970,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="5"/>
@@ -975,7 +979,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5"/>
@@ -984,7 +988,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
@@ -1003,7 +1007,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" s="5"/>
     </row>
@@ -1042,7 +1046,7 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="E25" s="5"/>
     </row>
@@ -1056,13 +1060,13 @@
     <row r="27" spans="1:5" ht="30">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E27" s="5"/>
     </row>
@@ -1070,7 +1074,7 @@
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="5"/>
@@ -1085,13 +1089,13 @@
     <row r="30" spans="1:5">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -1099,7 +1103,7 @@
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
@@ -1114,13 +1118,13 @@
     <row r="33" spans="1:5">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -1128,10 +1132,10 @@
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -1149,7 +1153,7 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -1160,7 +1164,7 @@
         <v>10</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -1168,10 +1172,10 @@
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -1189,7 +1193,7 @@
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -1203,11 +1207,11 @@
     <row r="42" spans="1:5">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -1221,11 +1225,11 @@
     <row r="44" spans="1:5">
       <c r="A44" s="1"/>
       <c r="B44" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -1233,7 +1237,7 @@
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="5"/>
@@ -1242,7 +1246,7 @@
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="5"/>
@@ -1251,7 +1255,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="5"/>
@@ -1260,7 +1264,7 @@
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="5"/>
@@ -1276,7 +1280,7 @@
       <c r="A50" s="1"/>
       <c r="B50" s="6"/>
       <c r="C50" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="5"/>
@@ -1284,10 +1288,10 @@
     <row r="51" spans="1:5">
       <c r="A51" s="1"/>
       <c r="B51" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="5"/>
@@ -1296,7 +1300,7 @@
       <c r="A52" s="1"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="5"/>
@@ -1305,7 +1309,7 @@
       <c r="A53" s="1"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="5"/>
@@ -1314,7 +1318,7 @@
       <c r="A54" s="1"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
@@ -1323,7 +1327,7 @@
       <c r="A55" s="1"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="5"/>
@@ -1332,10 +1336,10 @@
       <c r="A56" s="1"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E56" s="5"/>
     </row>
@@ -1343,10 +1347,10 @@
       <c r="A57" s="1"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E57" s="5"/>
     </row>
@@ -1354,10 +1358,10 @@
       <c r="A58" s="1"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E58" s="5"/>
     </row>
@@ -1365,10 +1369,10 @@
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E59" s="5"/>
     </row>
@@ -1376,10 +1380,10 @@
       <c r="A60" s="1"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D60" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="E60" s="5"/>
     </row>
@@ -1387,7 +1391,7 @@
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="5"/>
@@ -1396,10 +1400,10 @@
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E62" s="1"/>
     </row>
@@ -1407,10 +1411,10 @@
       <c r="A63" s="1"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E63" s="5"/>
     </row>
@@ -1418,10 +1422,10 @@
       <c r="A64" s="1"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E64" s="5"/>
     </row>
@@ -1429,10 +1433,10 @@
       <c r="A65" s="1"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E65" s="5"/>
     </row>
@@ -1486,13 +1490,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -1501,10 +1505,10 @@
         <v>10</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
@@ -2283,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2315,13 +2319,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -2330,10 +2334,10 @@
         <v>10</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
@@ -2352,7 +2356,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L2"/>
       <c r="M2"/>
@@ -2370,13 +2374,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="L3"/>
       <c r="M3"/>
@@ -2394,16 +2398,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L4"/>
       <c r="M4"/>
@@ -2421,19 +2425,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
@@ -2454,13 +2458,13 @@
         <v>10</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L6"/>
       <c r="M6"/>
@@ -2478,13 +2482,13 @@
         <v>10</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L7"/>
       <c r="M7"/>
@@ -2502,13 +2506,13 @@
         <v>10</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L8"/>
       <c r="M8"/>
@@ -2526,13 +2530,13 @@
         <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -2550,13 +2554,13 @@
         <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L10"/>
       <c r="M10"/>
@@ -2577,10 +2581,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="L11"/>
       <c r="M11"/>
@@ -2598,13 +2602,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="L12"/>
       <c r="M12"/>
@@ -2619,10 +2623,13 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="L13"/>
       <c r="M13"/>
@@ -2637,10 +2644,13 @@
     </row>
     <row r="14" spans="1:21" ht="30">
       <c r="A14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="L14"/>
       <c r="M14"/>
@@ -2661,7 +2671,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>16</v>
@@ -3091,6 +3101,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Partial implementation of row filtering
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="99">
   <si>
     <t>name</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>=</t>
-  </si>
-  <si>
-    <t>The value of another column</t>
   </si>
   <si>
     <t>Text enclosed in single quotation marks</t>
@@ -314,6 +311,15 @@
   </si>
   <si>
     <t xml:space="preserve">The name to be shown at the top of the colum in the report.  Can be any value. </t>
+  </si>
+  <si>
+    <t>The value of another column. This column can be in the data form in which case column name is also the question name.</t>
+  </si>
+  <si>
+    <t>An integer</t>
+  </si>
+  <si>
+    <t>A decimal</t>
   </si>
 </sst>
 </file>
@@ -382,8 +388,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -450,7 +458,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -467,6 +475,7 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -483,6 +492,7 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -812,14 +822,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="83.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -860,7 +871,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
@@ -912,10 +923,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="E10" s="5"/>
     </row>
@@ -923,10 +934,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="E11" s="5"/>
     </row>
@@ -970,7 +981,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="5"/>
@@ -979,7 +990,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5"/>
@@ -988,7 +999,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
@@ -1007,7 +1018,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E20" s="5"/>
     </row>
@@ -1046,7 +1057,7 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E25" s="5"/>
     </row>
@@ -1060,13 +1071,13 @@
     <row r="27" spans="1:5" ht="30">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="5"/>
     </row>
@@ -1074,7 +1085,7 @@
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="5"/>
@@ -1089,13 +1100,13 @@
     <row r="30" spans="1:5">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -1103,7 +1114,7 @@
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
@@ -1118,13 +1129,13 @@
     <row r="33" spans="1:5">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -1132,10 +1143,10 @@
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -1168,14 +1179,14 @@
       </c>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:5" ht="30">
+    <row r="38" spans="1:5">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -1211,7 +1222,7 @@
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -1225,11 +1236,11 @@
     <row r="44" spans="1:5">
       <c r="A44" s="1"/>
       <c r="B44" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -1237,7 +1248,7 @@
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="5"/>
@@ -1246,7 +1257,7 @@
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="5"/>
@@ -1255,7 +1266,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="5"/>
@@ -1264,7 +1275,7 @@
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="5"/>
@@ -1280,7 +1291,7 @@
       <c r="A50" s="1"/>
       <c r="B50" s="6"/>
       <c r="C50" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="5"/>
@@ -1288,7 +1299,7 @@
     <row r="51" spans="1:5">
       <c r="A51" s="1"/>
       <c r="B51" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>31</v>
@@ -1332,14 +1343,14 @@
       <c r="D55" s="6"/>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" ht="30">
       <c r="A56" s="1"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="E56" s="5"/>
     </row>
@@ -1347,10 +1358,10 @@
       <c r="A57" s="1"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E57" s="5"/>
     </row>
@@ -1358,10 +1369,10 @@
       <c r="A58" s="1"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="E58" s="5"/>
     </row>
@@ -1369,10 +1380,10 @@
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="E59" s="5"/>
     </row>
@@ -1380,10 +1391,10 @@
       <c r="A60" s="1"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E60" s="5"/>
     </row>
@@ -1391,54 +1402,76 @@
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D61" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E62" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="E62" s="5"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>83</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="D63" s="6"/>
       <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E64" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E65" s="5"/>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="1"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E66" s="5"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E67" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1490,13 +1523,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -1508,7 +1541,7 @@
         <v>28</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
@@ -2319,13 +2352,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -2337,7 +2370,7 @@
         <v>28</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
@@ -2407,7 +2440,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L4"/>
       <c r="M4"/>
@@ -2434,10 +2467,10 @@
         <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
@@ -2461,10 +2494,10 @@
         <v>30</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L6"/>
       <c r="M6"/>
@@ -2482,13 +2515,13 @@
         <v>10</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L7"/>
       <c r="M7"/>
@@ -2506,13 +2539,13 @@
         <v>10</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L8"/>
       <c r="M8"/>
@@ -2530,13 +2563,13 @@
         <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -2554,13 +2587,13 @@
         <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L10"/>
       <c r="M10"/>
@@ -2581,10 +2614,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="L11"/>
       <c r="M11"/>
@@ -2602,13 +2635,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="L12"/>
       <c r="M12"/>
@@ -2623,13 +2656,13 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L13"/>
       <c r="M13"/>
@@ -2644,13 +2677,13 @@
     </row>
     <row r="14" spans="1:21" ht="30">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L14"/>
       <c r="M14"/>
@@ -2671,7 +2704,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Update text on user_role
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-500" yWindow="260" windowWidth="25360" windowHeight="14040" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="13800" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>True if the column does not have a value</t>
   </si>
   <si>
-    <t>${_mgmt_action_deadline} is empty</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
@@ -320,6 +317,9 @@
   </si>
   <si>
     <t>If used after a select_one then the list of choices will be the users on the system that have the specified role.  Multiple rows with different roles can be added.   The name of the role goes in the "name" column</t>
+  </si>
+  <si>
+    <t>${_mgmt_action_deadline} empty</t>
   </si>
 </sst>
 </file>
@@ -824,7 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+    <sheetView topLeftCell="B3" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -923,10 +923,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E10" s="5"/>
     </row>
@@ -934,10 +934,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E11" s="5"/>
     </row>
@@ -981,7 +981,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="5"/>
@@ -990,7 +990,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5"/>
@@ -999,7 +999,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E20" s="5"/>
     </row>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E25" s="5"/>
     </row>
@@ -1071,13 +1071,13 @@
     <row r="27" spans="1:5" ht="30">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E27" s="5"/>
     </row>
@@ -1085,7 +1085,7 @@
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="5"/>
@@ -1100,13 +1100,13 @@
     <row r="30" spans="1:5">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -1114,7 +1114,7 @@
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
@@ -1129,13 +1129,13 @@
     <row r="33" spans="1:5">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -1143,10 +1143,10 @@
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -1183,10 +1183,10 @@
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -1236,11 +1236,11 @@
     <row r="44" spans="1:5">
       <c r="A44" s="1"/>
       <c r="B44" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -1248,7 +1248,7 @@
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="5"/>
@@ -1257,7 +1257,7 @@
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="5"/>
@@ -1266,7 +1266,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="5"/>
@@ -1275,7 +1275,7 @@
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="5"/>
@@ -1291,7 +1291,7 @@
       <c r="A50" s="1"/>
       <c r="B50" s="6"/>
       <c r="C50" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="5"/>
@@ -1350,7 +1350,7 @@
         <v>41</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E56" s="5"/>
     </row>
@@ -1369,10 +1369,10 @@
       <c r="A58" s="1"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E58" s="5"/>
     </row>
@@ -1380,10 +1380,10 @@
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E59" s="5"/>
     </row>
@@ -1402,7 +1402,7 @@
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>43</v>
@@ -1413,10 +1413,10 @@
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D62" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="E62" s="5"/>
     </row>
@@ -1424,7 +1424,7 @@
       <c r="A63" s="1"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="5"/>
@@ -1433,10 +1433,10 @@
       <c r="A64" s="1"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E64" s="1"/>
     </row>
@@ -1444,10 +1444,10 @@
       <c r="A65" s="1"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E65" s="5"/>
     </row>
@@ -1455,10 +1455,10 @@
       <c r="A66" s="1"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E66" s="5"/>
     </row>
@@ -1466,10 +1466,10 @@
       <c r="A67" s="1"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E67" s="5"/>
     </row>
@@ -1523,13 +1523,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -1541,7 +1541,7 @@
         <v>28</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
@@ -2320,8 +2320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2352,13 +2352,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -2370,7 +2370,7 @@
         <v>28</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
@@ -2440,7 +2440,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4"/>
       <c r="M4"/>
@@ -2467,10 +2467,10 @@
         <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
@@ -2494,10 +2494,10 @@
         <v>30</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L6"/>
       <c r="M6"/>
@@ -2518,10 +2518,10 @@
         <v>36</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L7"/>
       <c r="M7"/>
@@ -2542,10 +2542,10 @@
         <v>37</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L8"/>
       <c r="M8"/>
@@ -2563,13 +2563,13 @@
         <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -2587,13 +2587,13 @@
         <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L10"/>
       <c r="M10"/>
@@ -2614,10 +2614,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="L11"/>
       <c r="M11"/>
@@ -2635,13 +2635,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="L12"/>
       <c r="M12"/>
@@ -2656,13 +2656,13 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="J13" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L13"/>
       <c r="M13"/>
@@ -2677,13 +2677,13 @@
     </row>
     <row r="14" spans="1:21" ht="30">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L14"/>
       <c r="M14"/>
@@ -2704,7 +2704,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Update help link in smap editor for secondary pages
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="13800" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14020" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -425,7 +425,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -454,8 +454,23 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="35">
@@ -824,21 +839,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="83.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="15" customWidth="1"/>
+    <col min="4" max="4" width="83.33203125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5">
@@ -846,29 +861,29 @@
       <c r="B2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
@@ -876,10 +891,10 @@
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="5"/>
@@ -889,10 +904,10 @@
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="5"/>
@@ -900,10 +915,10 @@
     <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="5"/>
@@ -911,10 +926,10 @@
     <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="5"/>
@@ -922,10 +937,10 @@
     <row r="10" spans="1:5" ht="30">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="12" t="s">
         <v>96</v>
       </c>
       <c r="E10" s="5"/>
@@ -933,10 +948,10 @@
     <row r="11" spans="1:5" ht="45">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="12" t="s">
         <v>97</v>
       </c>
       <c r="E11" s="5"/>
@@ -944,8 +959,8 @@
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
@@ -953,62 +968,62 @@
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="150">
@@ -1016,8 +1031,8 @@
       <c r="B20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="12"/>
+      <c r="D20" s="12" t="s">
         <v>83</v>
       </c>
       <c r="E20" s="5"/>
@@ -1025,29 +1040,29 @@
     <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="30">
@@ -1055,8 +1070,8 @@
       <c r="B25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="12"/>
+      <c r="D25" s="12" t="s">
         <v>92</v>
       </c>
       <c r="E25" s="5"/>
@@ -1064,8 +1079,8 @@
     <row r="26" spans="1:5">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" ht="30">
@@ -1073,10 +1088,10 @@
       <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E27" s="5"/>
@@ -1084,17 +1099,17 @@
     <row r="28" spans="1:5">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5">
@@ -1102,10 +1117,10 @@
       <c r="B30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="12" t="s">
         <v>56</v>
       </c>
       <c r="E30" s="5"/>
@@ -1113,17 +1128,17 @@
     <row r="31" spans="1:5">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="12"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5">
@@ -1131,10 +1146,10 @@
       <c r="B33" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E33" s="5"/>
@@ -1142,10 +1157,10 @@
     <row r="34" spans="1:5">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E34" s="5"/>
@@ -1153,8 +1168,8 @@
     <row r="35" spans="1:5">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5">
@@ -1162,8 +1177,8 @@
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
+      <c r="C36" s="12"/>
+      <c r="D36" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E36" s="5"/>
@@ -1171,10 +1186,10 @@
     <row r="37" spans="1:5">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="12" t="s">
         <v>27</v>
       </c>
       <c r="E37" s="5"/>
@@ -1182,10 +1197,10 @@
     <row r="38" spans="1:5">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="12" t="s">
         <v>85</v>
       </c>
       <c r="E38" s="5"/>
@@ -1193,8 +1208,8 @@
     <row r="39" spans="1:5">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
@@ -1202,8 +1217,8 @@
       <c r="B40" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2" t="s">
+      <c r="C40" s="12"/>
+      <c r="D40" s="12" t="s">
         <v>29</v>
       </c>
       <c r="E40" s="5"/>
@@ -1211,8 +1226,8 @@
     <row r="41" spans="1:5">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5">
@@ -1220,8 +1235,8 @@
       <c r="B42" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2" t="s">
+      <c r="C42" s="12"/>
+      <c r="D42" s="12" t="s">
         <v>67</v>
       </c>
       <c r="E42" s="5"/>
@@ -1229,8 +1244,8 @@
     <row r="43" spans="1:5">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5">
@@ -1238,8 +1253,8 @@
       <c r="B44" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2" t="s">
+      <c r="C44" s="12"/>
+      <c r="D44" s="12" t="s">
         <v>66</v>
       </c>
       <c r="E44" s="5"/>
@@ -1247,53 +1262,53 @@
     <row r="45" spans="1:5">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="2"/>
+      <c r="D45" s="12"/>
       <c r="E45" s="5"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="2"/>
+      <c r="D46" s="12"/>
       <c r="E46" s="5"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="2"/>
+      <c r="D47" s="12"/>
       <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="2"/>
+      <c r="D48" s="12"/>
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
       <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="10"/>
+      <c r="D50" s="14"/>
       <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:5">
@@ -1301,55 +1316,55 @@
       <c r="B51" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D51" s="6"/>
+      <c r="D51" s="11"/>
       <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="6"/>
+      <c r="D52" s="11"/>
       <c r="E52" s="5"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D53" s="6"/>
+      <c r="D53" s="11"/>
       <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D54" s="6"/>
+      <c r="D54" s="11"/>
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D55" s="6"/>
+      <c r="D55" s="11"/>
       <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:5" ht="30">
       <c r="A56" s="1"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D56" s="11" t="s">
         <v>93</v>
       </c>
       <c r="E56" s="5"/>
@@ -1357,10 +1372,10 @@
     <row r="57" spans="1:5">
       <c r="A57" s="1"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E57" s="5"/>
@@ -1368,10 +1383,10 @@
     <row r="58" spans="1:5">
       <c r="A58" s="1"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="11" t="s">
         <v>94</v>
       </c>
       <c r="E58" s="5"/>
@@ -1379,10 +1394,10 @@
     <row r="59" spans="1:5">
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="11" t="s">
         <v>95</v>
       </c>
       <c r="E59" s="5"/>
@@ -1390,10 +1405,10 @@
     <row r="60" spans="1:5">
       <c r="A60" s="1"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E60" s="5"/>
@@ -1401,10 +1416,10 @@
     <row r="61" spans="1:5">
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E61" s="5"/>
@@ -1412,10 +1427,10 @@
     <row r="62" spans="1:5">
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="11" t="s">
         <v>45</v>
       </c>
       <c r="E62" s="5"/>
@@ -1423,19 +1438,19 @@
     <row r="63" spans="1:5">
       <c r="A63" s="1"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D63" s="6"/>
+      <c r="D63" s="11"/>
       <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D64" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E64" s="1"/>
@@ -1443,10 +1458,10 @@
     <row r="65" spans="1:5">
       <c r="A65" s="1"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D65" s="11" t="s">
         <v>80</v>
       </c>
       <c r="E65" s="5"/>
@@ -1454,10 +1469,10 @@
     <row r="66" spans="1:5">
       <c r="A66" s="1"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="11" t="s">
         <v>81</v>
       </c>
       <c r="E66" s="5"/>
@@ -1465,10 +1480,10 @@
     <row r="67" spans="1:5">
       <c r="A67" s="1"/>
       <c r="B67" s="6"/>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D67" s="11" t="s">
         <v>82</v>
       </c>
       <c r="E67" s="5"/>
@@ -2320,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2658,12 +2673,13 @@
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="D13" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="J13" s="8"/>
       <c r="L13"/>
       <c r="M13"/>
       <c r="N13"/>
@@ -2679,11 +2695,11 @@
       <c r="A14" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="L14"/>
       <c r="M14"/>

</xml_diff>

<commit_message>
Added action columns to oversight spreadsheet
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14020" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="112">
   <si>
     <t>name</t>
   </si>
@@ -320,13 +320,74 @@
   </si>
   <si>
     <t>${_mgmt_action_deadline} empty</t>
+  </si>
+  <si>
+    <t>ident</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>sms</t>
+  </si>
+  <si>
+    <r>
+      <t>Leave empty if the person to be notified is identified by the value set in this column. Otherwise enter an ident,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> email address or phone number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>notify type</t>
+  </si>
+  <si>
+    <t>notify person</t>
+  </si>
+  <si>
+    <t>Future - not yet supported</t>
+  </si>
+  <si>
+    <t>An action should be taken when the value of this column changes</t>
+  </si>
+  <si>
+    <t>The following columns specify actions that should be taken when the column changes.  The "row type" needs to be "action"</t>
+  </si>
+  <si>
+    <t>respond</t>
+  </si>
+  <si>
+    <t>Only "ident" is currently supported</t>
+  </si>
+  <si>
+    <t>Currently only "respond" is supported. This will request the notified user to use the management form to update the record</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -358,8 +419,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,6 +443,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,7 +499,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -466,11 +540,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="35">
@@ -837,16 +920,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="18.5" style="15" customWidth="1"/>
-    <col min="4" max="4" width="83.33203125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="14" customWidth="1"/>
+    <col min="4" max="4" width="83.33203125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -959,26 +1043,28 @@
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="C12" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>107</v>
+      </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C14" s="12" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="5"/>
@@ -987,7 +1073,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="5"/>
@@ -996,7 +1082,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="12" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="5"/>
@@ -1005,7 +1091,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="12" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="5"/>
@@ -1014,7 +1100,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="5"/>
@@ -1022,26 +1108,28 @@
     <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="12"/>
+      <c r="C19" s="12" t="s">
+        <v>74</v>
+      </c>
       <c r="D19" s="12"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="150">
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" ht="150">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12" t="s">
+      <c r="C21" s="12"/>
+      <c r="D21" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5">
@@ -1065,132 +1153,128 @@
       <c r="D24" s="12"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="30">
+    <row r="25" spans="1:5">
       <c r="A25" s="1"/>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" ht="30">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12" t="s">
+      <c r="C26" s="12"/>
+      <c r="D26" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="30">
+    <row r="27" spans="1:5">
       <c r="A27" s="1"/>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" ht="30">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C28" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D28" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="12"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="12"/>
+      <c r="C29" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="D29" s="12"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1"/>
-      <c r="B30" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="C31" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="12"/>
+        <v>52</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="12"/>
+      <c r="C32" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="D32" s="12"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1"/>
-      <c r="B33" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>71</v>
-      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="C34" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="C35" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>72</v>
+      </c>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1"/>
-      <c r="B36" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B36" s="2"/>
       <c r="C36" s="12"/>
-      <c r="D36" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="D36" s="12"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="B37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="12"/>
       <c r="D37" s="12" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -1198,81 +1282,83 @@
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="12" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
+      <c r="C39" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>85</v>
+      </c>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1"/>
-      <c r="B40" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B40" s="2"/>
       <c r="C40" s="12"/>
-      <c r="D40" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="D40" s="12"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1"/>
-      <c r="B41" s="2"/>
+      <c r="B41" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
+      <c r="D41" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1"/>
-      <c r="B42" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="B42" s="2"/>
       <c r="C42" s="12"/>
-      <c r="D42" s="12" t="s">
-        <v>67</v>
-      </c>
+      <c r="D42" s="12"/>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
+      <c r="B43" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="D43" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1"/>
-      <c r="B44" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="B44" s="2"/>
       <c r="C44" s="12"/>
-      <c r="D44" s="12" t="s">
-        <v>66</v>
-      </c>
+      <c r="D44" s="12"/>
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D45" s="12"/>
+      <c r="B45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12" t="s">
+        <v>66</v>
+      </c>
       <c r="E45" s="5"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="5"/>
@@ -1281,7 +1367,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="5"/>
@@ -1290,7 +1376,7 @@
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="5"/>
@@ -1298,148 +1384,144 @@
     <row r="49" spans="1:5">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
-      <c r="C49" s="12"/>
+      <c r="C49" s="12" t="s">
+        <v>60</v>
+      </c>
       <c r="D49" s="12"/>
       <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50" s="14"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="1"/>
-      <c r="B51" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D51" s="11"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18" t="s">
+        <v>108</v>
+      </c>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" ht="30">
       <c r="A52" s="1"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D52" s="11"/>
+      <c r="B52" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>111</v>
+      </c>
       <c r="E52" s="5"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D53" s="11"/>
+      <c r="B53" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>110</v>
+      </c>
       <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="11"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>106</v>
+      </c>
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D55" s="11"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>106</v>
+      </c>
       <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:5" ht="30">
       <c r="A56" s="1"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>93</v>
+      <c r="B56" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12" t="s">
+        <v>102</v>
       </c>
       <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>35</v>
-      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
       <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>94</v>
-      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
       <c r="E58" s="5"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>95</v>
-      </c>
+      <c r="C59" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D59" s="15"/>
       <c r="E59" s="5"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1"/>
-      <c r="B60" s="6"/>
+      <c r="B60" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="C60" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>42</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D60" s="11"/>
       <c r="E60" s="5"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
       <c r="C61" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>43</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D61" s="11"/>
       <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
       <c r="C62" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>45</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D62" s="11"/>
       <c r="E62" s="5"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1"/>
       <c r="B63" s="6"/>
       <c r="C63" s="11" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="D63" s="11"/>
       <c r="E63" s="5"/>
@@ -1448,21 +1530,19 @@
       <c r="A64" s="1"/>
       <c r="B64" s="6"/>
       <c r="C64" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E64" s="1"/>
-    </row>
-    <row r="65" spans="1:5">
+        <v>34</v>
+      </c>
+      <c r="D64" s="11"/>
+      <c r="E64" s="5"/>
+    </row>
+    <row r="65" spans="1:5" ht="30">
       <c r="A65" s="1"/>
       <c r="B65" s="6"/>
       <c r="C65" s="11" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="E65" s="5"/>
     </row>
@@ -1470,10 +1550,10 @@
       <c r="A66" s="1"/>
       <c r="B66" s="6"/>
       <c r="C66" s="11" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="E66" s="5"/>
     </row>
@@ -1481,16 +1561,113 @@
       <c r="A67" s="1"/>
       <c r="B67" s="6"/>
       <c r="C67" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E67" s="5"/>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="1"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E68" s="5"/>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E69" s="5"/>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="1"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="1"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E71" s="5"/>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="1"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D72" s="11"/>
+      <c r="E72" s="5"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="1"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="1"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E74" s="5"/>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="1"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E75" s="5"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="1"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D76" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E67" s="5"/>
+      <c r="E76" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C59:D59"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1506,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1519,7 +1696,8 @@
     <col min="8" max="8" width="10.83203125" style="1"/>
     <col min="9" max="9" width="32.83203125" style="1" customWidth="1"/>
     <col min="10" max="11" width="17.6640625" style="1" customWidth="1"/>
-    <col min="12" max="14" width="10.83203125" style="1"/>
+    <col min="12" max="13" width="10.83203125" style="1"/>
+    <col min="14" max="14" width="17" style="1" customWidth="1"/>
     <col min="15" max="15" width="75.6640625" style="1" customWidth="1"/>
     <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -1558,9 +1736,15 @@
       <c r="K1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1"/>
+      <c r="L1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="O1"/>
       <c r="P1"/>
     </row>
@@ -2335,7 +2519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add roles to temporary actions
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="114">
   <si>
     <t>name</t>
   </si>
@@ -381,6 +381,12 @@
   </si>
   <si>
     <t>Currently only "respond" is supported. This will request the notified user to use the management form to update the record</t>
+  </si>
+  <si>
+    <t>roles</t>
+  </si>
+  <si>
+    <t>A comma separated list of roles that should be given to the user to respond to the action</t>
   </si>
 </sst>
 </file>
@@ -543,9 +549,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -554,6 +557,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="35">
@@ -922,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1399,9 +1405,9 @@
     </row>
     <row r="51" spans="1:5" ht="30">
       <c r="A51" s="1"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18" t="s">
+      <c r="B51" s="16"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17" t="s">
         <v>108</v>
       </c>
       <c r="E51" s="5"/>
@@ -1438,7 +1444,7 @@
       <c r="C54" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="D54" s="15" t="s">
         <v>106</v>
       </c>
       <c r="E54" s="5"/>
@@ -1449,7 +1455,7 @@
       <c r="C55" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="15" t="s">
         <v>106</v>
       </c>
       <c r="E55" s="5"/>
@@ -1467,9 +1473,13 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1"/>
-      <c r="B57" s="2"/>
+      <c r="B57" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
+      <c r="D57" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:5">
@@ -1482,10 +1492,10 @@
     <row r="59" spans="1:5">
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="15" t="s">
+      <c r="C59" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D59" s="15"/>
+      <c r="D59" s="18"/>
       <c r="E59" s="5"/>
     </row>
     <row r="60" spans="1:5">

</xml_diff>

<commit_message>
Removed none from XLS export. Added + integer to oversight template
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="116">
   <si>
     <t>name</t>
   </si>
@@ -281,9 +281,6 @@
   </si>
   <si>
     <t xml:space="preserve">An expression, see below for what can be included in an expresion. </t>
-  </si>
-  <si>
-    <t>All of the following tokens should be separated by spaces. For exampe ( 100 + 5 ) / 10</t>
   </si>
   <si>
     <t>Deadline Met</t>
@@ -387,6 +384,15 @@
   </si>
   <si>
     <t>A comma separated list of roles that should be given to the user to respond to the action</t>
+  </si>
+  <si>
+    <t>All of the following tokens should be separated by spaces. For example ( 100 + 5 ) / 10</t>
+  </si>
+  <si>
+    <t>+ integer {nn}</t>
+  </si>
+  <si>
+    <t>Adds nn days to a date.  nn being an integer value</t>
   </si>
 </sst>
 </file>
@@ -934,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77:XFD77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1039,7 +1045,7 @@
         <v>62</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E10" s="5"/>
     </row>
@@ -1047,10 +1053,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E11" s="5"/>
     </row>
@@ -1058,10 +1064,10 @@
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12" s="5"/>
     </row>
@@ -1181,7 +1187,7 @@
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E26" s="5"/>
     </row>
@@ -1416,33 +1422,33 @@
       <c r="B51" s="16"/>
       <c r="C51" s="17"/>
       <c r="D51" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:5" ht="30">
       <c r="A52" s="1"/>
       <c r="B52" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E52" s="5"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1"/>
       <c r="B53" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E53" s="5"/>
     </row>
@@ -1450,10 +1456,10 @@
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="C54" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E54" s="5"/>
     </row>
@@ -1461,32 +1467,32 @@
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="C55" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:5" ht="30">
       <c r="A56" s="1"/>
       <c r="B56" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C56" s="12"/>
       <c r="D56" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1"/>
       <c r="B57" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C57" s="12"/>
       <c r="D57" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E57" s="5"/>
     </row>
@@ -1501,7 +1507,7 @@
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
       <c r="C59" s="18" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="D59" s="18"/>
       <c r="E59" s="5"/>
@@ -1560,7 +1566,7 @@
         <v>41</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E65" s="5"/>
     </row>
@@ -1582,7 +1588,7 @@
         <v>73</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E67" s="5"/>
     </row>
@@ -1593,7 +1599,7 @@
         <v>74</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E68" s="5"/>
     </row>
@@ -1682,6 +1688,17 @@
         <v>82</v>
       </c>
       <c r="E76" s="5"/>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="1"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E77" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1701,7 +1718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
@@ -1755,16 +1772,16 @@
         <v>65</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="O1" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P1"/>
     </row>
@@ -2713,7 +2730,7 @@
         <v>30</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>57</v>
@@ -2737,7 +2754,7 @@
         <v>36</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>58</v>
@@ -2761,7 +2778,7 @@
         <v>37</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>59</v>
@@ -2782,10 +2799,10 @@
         <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>59</v>
@@ -2809,7 +2826,7 @@
         <v>44</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Added ability to add an integer number of days from todays date
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="118">
   <si>
     <t>name</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t xml:space="preserve">${column} </t>
-  </si>
-  <si>
-    <t>Current data and time</t>
   </si>
   <si>
     <t>True if the column does not have a value</t>
@@ -393,6 +390,15 @@
   </si>
   <si>
     <t>Adds nn days to a date.  nn being an integer value</t>
+  </si>
+  <si>
+    <t>current_date</t>
+  </si>
+  <si>
+    <t>Current date</t>
+  </si>
+  <si>
+    <t>Current date and time</t>
   </si>
 </sst>
 </file>
@@ -940,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:XFD77"/>
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1042,10 +1048,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E10" s="5"/>
     </row>
@@ -1053,10 +1059,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E11" s="5"/>
     </row>
@@ -1064,10 +1070,10 @@
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E12" s="5"/>
     </row>
@@ -1111,7 +1117,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="5"/>
@@ -1120,7 +1126,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="5"/>
@@ -1129,7 +1135,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="5"/>
@@ -1148,7 +1154,7 @@
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E21" s="5"/>
     </row>
@@ -1187,7 +1193,7 @@
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" s="5"/>
     </row>
@@ -1201,13 +1207,13 @@
     <row r="28" spans="1:5" ht="30">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>52</v>
-      </c>
       <c r="D28" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -1215,7 +1221,7 @@
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="5"/>
@@ -1230,13 +1236,13 @@
     <row r="31" spans="1:5">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -1244,7 +1250,7 @@
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="5"/>
@@ -1259,13 +1265,13 @@
     <row r="34" spans="1:5">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>71</v>
       </c>
       <c r="E34" s="5"/>
     </row>
@@ -1273,10 +1279,10 @@
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -1313,10 +1319,10 @@
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="C39" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>85</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -1352,7 +1358,7 @@
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -1366,11 +1372,11 @@
     <row r="45" spans="1:5">
       <c r="A45" s="1"/>
       <c r="B45" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -1378,7 +1384,7 @@
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="5"/>
@@ -1387,7 +1393,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="5"/>
@@ -1396,7 +1402,7 @@
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="5"/>
@@ -1405,7 +1411,7 @@
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="C49" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="5"/>
@@ -1422,33 +1428,33 @@
       <c r="B51" s="16"/>
       <c r="C51" s="17"/>
       <c r="D51" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:5" ht="30">
       <c r="A52" s="1"/>
       <c r="B52" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E52" s="5"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1"/>
       <c r="B53" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E53" s="5"/>
     </row>
@@ -1456,10 +1462,10 @@
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="C54" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E54" s="5"/>
     </row>
@@ -1467,32 +1473,32 @@
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="C55" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:5" ht="30">
       <c r="A56" s="1"/>
       <c r="B56" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C56" s="12"/>
       <c r="D56" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1"/>
       <c r="B57" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C57" s="12"/>
       <c r="D57" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E57" s="5"/>
     </row>
@@ -1507,7 +1513,7 @@
       <c r="A59" s="1"/>
       <c r="B59" s="6"/>
       <c r="C59" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D59" s="18"/>
       <c r="E59" s="5"/>
@@ -1566,7 +1572,7 @@
         <v>41</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E65" s="5"/>
     </row>
@@ -1585,10 +1591,10 @@
       <c r="A67" s="1"/>
       <c r="B67" s="6"/>
       <c r="C67" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E67" s="5"/>
     </row>
@@ -1596,10 +1602,10 @@
       <c r="A68" s="1"/>
       <c r="B68" s="6"/>
       <c r="C68" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E68" s="5"/>
     </row>
@@ -1610,7 +1616,7 @@
         <v>38</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="E69" s="5"/>
     </row>
@@ -1618,10 +1624,10 @@
       <c r="A70" s="1"/>
       <c r="B70" s="6"/>
       <c r="C70" s="11" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="E70" s="5"/>
     </row>
@@ -1629,10 +1635,10 @@
       <c r="A71" s="1"/>
       <c r="B71" s="6"/>
       <c r="C71" s="11" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E71" s="5"/>
     </row>
@@ -1640,21 +1646,21 @@
       <c r="A72" s="1"/>
       <c r="B72" s="6"/>
       <c r="C72" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D72" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="E72" s="5"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="1"/>
       <c r="B73" s="6"/>
       <c r="C73" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E73" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="D73" s="11"/>
+      <c r="E73" s="5"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="1"/>
@@ -1663,18 +1669,18 @@
         <v>75</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E74" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1"/>
       <c r="B75" s="6"/>
       <c r="C75" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E75" s="5"/>
     </row>
@@ -1682,10 +1688,10 @@
       <c r="A76" s="1"/>
       <c r="B76" s="6"/>
       <c r="C76" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E76" s="5"/>
     </row>
@@ -1693,12 +1699,23 @@
       <c r="A77" s="1"/>
       <c r="B77" s="6"/>
       <c r="C77" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E77" s="5"/>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="1"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D78" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D77" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E77" s="5"/>
+      <c r="E78" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1751,13 +1768,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -1769,19 +1786,19 @@
         <v>28</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>104</v>
-      </c>
       <c r="O1" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P1"/>
     </row>
@@ -2588,13 +2605,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -2606,7 +2623,7 @@
         <v>28</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
@@ -2676,7 +2693,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L4"/>
       <c r="M4"/>
@@ -2703,10 +2720,10 @@
         <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
@@ -2730,10 +2747,10 @@
         <v>30</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L6"/>
       <c r="M6"/>
@@ -2754,10 +2771,10 @@
         <v>36</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L7"/>
       <c r="M7"/>
@@ -2778,10 +2795,10 @@
         <v>37</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L8"/>
       <c r="M8"/>
@@ -2799,13 +2816,13 @@
         <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -2823,13 +2840,13 @@
         <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L10"/>
       <c r="M10"/>
@@ -2850,10 +2867,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="L11"/>
       <c r="M11"/>
@@ -2871,13 +2888,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="L12"/>
       <c r="M12"/>
@@ -2892,13 +2909,13 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="J13" s="8"/>
       <c r="L13"/>
@@ -2914,13 +2931,13 @@
     </row>
     <row r="14" spans="1:21" ht="30">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L14"/>
       <c r="M14"/>
@@ -2941,7 +2958,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Update smapServer to 19.08
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="142">
   <si>
     <t>name</t>
   </si>
@@ -386,12 +386,6 @@
     <t>All of the following tokens should be separated by spaces. For example ( 100 + 5 ) / 10</t>
   </si>
   <si>
-    <t>+ integer {nn}</t>
-  </si>
-  <si>
-    <t>Adds nn days to a date.  nn being an integer value</t>
-  </si>
-  <si>
     <t>current_date</t>
   </si>
   <si>
@@ -423,6 +417,60 @@
   </si>
   <si>
     <t>Use when the source question is of type image, this will identify objects within the image to add as labels</t>
+  </si>
+  <si>
+    <t>{1_day}</t>
+  </si>
+  <si>
+    <t>(n_days}</t>
+  </si>
+  <si>
+    <t>{1_hour}</t>
+  </si>
+  <si>
+    <t>{n_hours}</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by 1 day</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by n days</t>
+  </si>
+  <si>
+    <t>{1_minute}</t>
+  </si>
+  <si>
+    <t>{n_minutes}</t>
+  </si>
+  <si>
+    <t>{1_second}</t>
+  </si>
+  <si>
+    <t>{n_seconds}</t>
+  </si>
+  <si>
+    <t>{hh:mm:ss}</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time byhh hours mm minutes and ss seconds</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by n seconds</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by 1second</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by n minutes</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by 1 minute</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by n hours</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by 1 hour</t>
   </si>
 </sst>
 </file>
@@ -504,8 +552,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -604,7 +670,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -625,6 +691,15 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -645,6 +720,15 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -974,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83:D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1454,11 +1538,11 @@
     <row r="51" spans="1:5">
       <c r="A51" s="1"/>
       <c r="B51" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E51" s="5"/>
     </row>
@@ -1466,10 +1550,10 @@
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E52" s="5"/>
     </row>
@@ -1477,10 +1561,10 @@
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="C53" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E53" s="5"/>
     </row>
@@ -1488,10 +1572,10 @@
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="C54" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E54" s="5"/>
     </row>
@@ -1695,7 +1779,7 @@
         <v>38</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E74" s="5"/>
     </row>
@@ -1703,10 +1787,10 @@
       <c r="A75" s="1"/>
       <c r="B75" s="6"/>
       <c r="C75" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E75" s="5"/>
     </row>
@@ -1786,15 +1870,85 @@
       <c r="E82" s="5"/>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="1"/>
       <c r="B83" s="6"/>
       <c r="C83" s="11" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="E83" s="5"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="B84" s="6"/>
+      <c r="C84" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="B85" s="6"/>
+      <c r="C85" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="B86" s="6"/>
+      <c r="C86" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="B87" s="6"/>
+      <c r="C87" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="B88" s="6"/>
+      <c r="C88" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="B89" s="6"/>
+      <c r="C89" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="B90" s="6"/>
+      <c r="C90" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="B91" s="6"/>
+      <c r="C91" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>135</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1814,9 +1968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1880,7 +2032,7 @@
         <v>110</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -2654,9 +2806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2668,11 +2818,11 @@
     <col min="9" max="9" width="32.83203125" style="1" customWidth="1"/>
     <col min="10" max="11" width="17.6640625" style="1" customWidth="1"/>
     <col min="12" max="14" width="10.83203125" style="1"/>
-    <col min="15" max="15" width="75.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" style="1" customWidth="1"/>
     <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" ht="30">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2706,11 +2856,21 @@
       <c r="K1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1"/>
-      <c r="O1"/>
-      <c r="P1"/>
+      <c r="L1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">

</xml_diff>